<commit_message>
First draft layout of HV circuit. Things to refine: (1) ground return pads / mounting holes for gnd return. (2) Idea of how the high voltage inputs/outputs actually hook up to the LAPPD and incoming cables. (3) UL796 standard has 1.6kV/mm rating on distances between conductors. Is this tolerance actually OK, considering the present layout of gnd pour. (4) Do all of the components clear mechanical constraints of the LAPPD and Ultem frame, i.e. we wont have a solder mound where the detector or frame needs to be flush.
</commit_message>
<xml_diff>
--- a/BOM/11-29-2022.xlsx
+++ b/BOM/11-29-2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejangelico/Documents/Stanford/LAPPD/Anodes/samtec-adapter-v2a/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejangelico/Documents/Stanford/LAPPD/Anodes/stripline-anode-capacitive-readout/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C87F40-8842-EC46-AF8C-C0395CB415D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9220CC62-00D1-3B44-8A27-31238334B505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="500" windowWidth="25600" windowHeight="16260" xr2:uid="{F2077957-3B34-F443-BA74-5CFAF79BDB72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -65,12 +65,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>here</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -87,81 +81,6 @@
   </si>
   <si>
     <t>spare per board</t>
-  </si>
-  <si>
-    <t>QPC6064</t>
-  </si>
-  <si>
-    <t>RFMW</t>
-  </si>
-  <si>
-    <t>SP6T RF switch</t>
-  </si>
-  <si>
-    <t>QP1, QP2, QP3, QP4, QP5</t>
-  </si>
-  <si>
-    <t>J1, J2, J3, J4, J5</t>
-  </si>
-  <si>
-    <t>SW1, SW2, SW3, SW4, SW5</t>
-  </si>
-  <si>
-    <t>3-position dip switch</t>
-  </si>
-  <si>
-    <t>76SB03T</t>
-  </si>
-  <si>
-    <t>GH7168-ND</t>
-  </si>
-  <si>
-    <t>Conn_Coaxial</t>
-  </si>
-  <si>
-    <t>SMA right angle</t>
-  </si>
-  <si>
-    <t>17-5-1814400-2CT-ND</t>
-  </si>
-  <si>
-    <t>Jumper</t>
-  </si>
-  <si>
-    <t>Battery holder</t>
-  </si>
-  <si>
-    <t>A144288-ND</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>TSV diode (transient suppression)</t>
-  </si>
-  <si>
-    <t>GSOT05C-E3-08CT-ND</t>
-  </si>
-  <si>
-    <t>TS1</t>
-  </si>
-  <si>
-    <t>1528-2553-ND</t>
-  </si>
-  <si>
-    <t>Switched barrel connector</t>
-  </si>
-  <si>
-    <t>450-1567-ND</t>
-  </si>
-  <si>
-    <t>Battery disconnect switch</t>
-  </si>
-  <si>
-    <t>BSW</t>
-  </si>
-  <si>
-    <t>PEXT</t>
   </si>
   <si>
     <t>Samtec QRM078</t>
@@ -539,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CF9324-42B4-FB42-9994-120323B15401}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,10 +486,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -579,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -600,182 +519,51 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D3">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M3" s="1"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D4">
-        <v>3.75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M4" s="1"/>
       <c r="O4" s="3">
         <v>44275</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D5">
-        <v>5.33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M5" s="1"/>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
       <c r="M6" s="1"/>
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M7" s="1"/>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D8">
-        <v>0.41</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M8" s="1"/>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D9">
-        <v>0.86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M9" s="1"/>
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D10">
-        <v>1.5</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="M10" s="1"/>
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -860,7 +648,7 @@
     </row>
     <row r="31" spans="7:15" x14ac:dyDescent="0.2">
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="7:15" x14ac:dyDescent="0.2">
@@ -870,15 +658,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M5" r:id="rId1" xr:uid="{14E5E7E0-90EF-C646-88C9-D41B5267D280}"/>
-    <hyperlink ref="M4" r:id="rId2" xr:uid="{A980B62A-6118-E04C-8649-F9B48CFA4BD6}"/>
-    <hyperlink ref="M3" r:id="rId3" xr:uid="{2612F521-1D22-7F49-8CC3-3A28C5C6039F}"/>
-    <hyperlink ref="M7" r:id="rId4" xr:uid="{400E5415-3EA8-2A47-8BF8-015C7FEB4FDA}"/>
-    <hyperlink ref="M8" r:id="rId5" xr:uid="{0EEDBD4A-3545-A041-9E4D-DE2818E7F991}"/>
-    <hyperlink ref="M10" r:id="rId6" xr:uid="{7E6793E3-7AAE-2947-A492-635DC319A73E}"/>
-    <hyperlink ref="M9" r:id="rId7" xr:uid="{46864AFC-FA27-F34E-B8C6-B4141955431B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A close to final version of high voltage circuitry, after having decided to go with SHV cable ends soldered on to SMD pads, potted, and strain relieved by zip ties. Also added SMA ports. This is one day before meeting to review
</commit_message>
<xml_diff>
--- a/BOM/11-29-2022.xlsx
+++ b/BOM/11-29-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejangelico/Documents/Stanford/LAPPD/Anodes/stripline-anode-capacitive-readout/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9220CC62-00D1-3B44-8A27-31238334B505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E69E97-F8EE-084F-95EE-0D8D0B58AE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="500" windowWidth="25600" windowHeight="16260" xr2:uid="{F2077957-3B34-F443-BA74-5CFAF79BDB72}"/>
+    <workbookView xWindow="6780" yWindow="23540" windowWidth="28800" windowHeight="16260" xr2:uid="{F2077957-3B34-F443-BA74-5CFAF79BDB72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,72 @@
   </si>
   <si>
     <t>Samtec QRM078</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>660-HV733ATTE3004F</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>For example, 2512 package type HV resistors</t>
+  </si>
+  <si>
+    <t>100 pF</t>
+  </si>
+  <si>
+    <t>SMD HV resistor, 2512</t>
+  </si>
+  <si>
+    <t>581-1812HA101k</t>
+  </si>
+  <si>
+    <t>10 nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD HV cap, 2220 </t>
+  </si>
+  <si>
+    <t>SMD HV cap, 1812</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>80-C2220C103KHR</t>
+  </si>
+  <si>
+    <t>200V SMD Zener</t>
+  </si>
+  <si>
+    <t>D_SOD123</t>
+  </si>
+  <si>
+    <t>200V Zener</t>
+  </si>
+  <si>
+    <t>78-BZD27C200P-HE3-08</t>
+  </si>
+  <si>
+    <t>0.1 uF</t>
+  </si>
+  <si>
+    <t>SMD gnd cap, 1812</t>
+  </si>
+  <si>
+    <t>Angled SMD SMA Jack</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>142-0711-271</t>
   </si>
 </sst>
 </file>
@@ -160,7 +226,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -448,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -459,7 +525,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,6 +592,9 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
@@ -533,29 +602,131 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M3" s="1"/>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M4" s="1"/>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O4" s="3">
         <v>44275</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M5" s="1"/>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M6" s="1"/>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M7" s="1"/>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M8" s="1"/>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -658,6 +829,14 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{261AB411-E9BB-3B48-86AB-54E42CFB6526}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{32C13E35-7325-224A-8477-BCBC82C5F937}"/>
+    <hyperlink ref="M5" r:id="rId3" xr:uid="{CD36EBDB-1CC0-AC4C-9425-1AC4FB5B560C}"/>
+    <hyperlink ref="M6" r:id="rId4" xr:uid="{8895AB7B-BE70-DB41-B7E6-79F8DDA396BF}"/>
+    <hyperlink ref="M7" r:id="rId5" xr:uid="{615D5860-4E34-634C-9216-EEF016CC4A24}"/>
+    <hyperlink ref="M8" r:id="rId6" xr:uid="{BEC14091-6465-8F43-9D5B-6B982553A9F1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>